<commit_message>
improvement of the nsp3 domain classifer
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV/domains_and_infos_of_nsp3.xlsx
@@ -9,17 +9,19 @@
   <sheets>
     <sheet name="nsp3_Ubl1" sheetId="1" r:id="rId1"/>
     <sheet name="nsp3_PL2pro" sheetId="2" r:id="rId2"/>
-    <sheet name="nsp3_SUD" sheetId="3" r:id="rId3"/>
-    <sheet name="nsp3_NAB" sheetId="4" r:id="rId4"/>
-    <sheet name="nsp3_Macro1" sheetId="5" r:id="rId5"/>
-    <sheet name="nsp3_Ubl2" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_Ubl2" sheetId="3" r:id="rId3"/>
+    <sheet name="nsp3_SUD" sheetId="4" r:id="rId4"/>
+    <sheet name="nsp3_NAB" sheetId="5" r:id="rId5"/>
+    <sheet name="nsp3_sec_btwn_Macro1_SUD" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_Macro1" sheetId="7" r:id="rId7"/>
+    <sheet name="nsp3_frgmnt_btwn_PL2pro_NAB" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
   <si>
     <t>PDB</t>
   </si>
@@ -60,6 +62,15 @@
     <t>2020-05-02</t>
   </si>
   <si>
+    <t>2w2g</t>
+  </si>
+  <si>
+    <t>HUMAN SARS CORONAVIRUS UNIQUE DOMAIN</t>
+  </si>
+  <si>
+    <t>2008-10-30</t>
+  </si>
+  <si>
     <t>2idy</t>
   </si>
   <si>
@@ -84,6 +95,66 @@
     <t>2016-10-10</t>
   </si>
   <si>
+    <t>3mj5</t>
+  </si>
+  <si>
+    <t>SEVERE ACUTE RESPIRATORY SYNDROME-CORONAVIRUS PAPAIN-LIKE PROTEASE INHIBITORS: DESIGN, SYNTHESIS, PROTEIN-LIGAND X-RAY STRUCTURE AND BIOLOGICAL EVALUATION</t>
+  </si>
+  <si>
+    <t>2010-04-12</t>
+  </si>
+  <si>
+    <t>5y3q</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE CONJUGATED WITH BETA-MERCAPTOETHANOL</t>
+  </si>
+  <si>
+    <t>2017-07-29</t>
+  </si>
+  <si>
+    <t>2fe8</t>
+  </si>
+  <si>
+    <t>SARS CORONAVIRUS PAPAIN-LIKE PROTEASE: STRUCTURE OF A VIRAL DEUBIQUITINATING ENZYME</t>
+  </si>
+  <si>
+    <t>2005-12-15</t>
+  </si>
+  <si>
+    <t>5y3e</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE IN COMPLEX WITH GLYCEROL</t>
+  </si>
+  <si>
+    <t>2017-07-28</t>
+  </si>
+  <si>
+    <t>5e6j</t>
+  </si>
+  <si>
+    <t>STRUCTURE OF SARS PLPRO BOUND TO A LYS48-LINKED DI-UBIQUITIN ACTIVITY BASED PROBE</t>
+  </si>
+  <si>
+    <t>2015-10-09</t>
+  </si>
+  <si>
+    <t>4mm3</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH UBIQUITIN ALDEHYDE</t>
+  </si>
+  <si>
+    <t>2013-09-08</t>
+  </si>
+  <si>
+    <t>5tl7</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH C- TERMINAL DOMAIN MOUSE ISG15</t>
+  </si>
+  <si>
     <t>3e9s</t>
   </si>
   <si>
@@ -102,70 +173,28 @@
     <t>2014-01-27</t>
   </si>
   <si>
-    <t>3mj5</t>
-  </si>
-  <si>
-    <t>SEVERE ACUTE RESPIRATORY SYNDROME-CORONAVIRUS PAPAIN-LIKE PROTEASE INHIBITORS: DESIGN, SYNTHESIS, PROTEIN-LIGAND X-RAY STRUCTURE AND BIOLOGICAL EVALUATION</t>
-  </si>
-  <si>
-    <t>2010-04-12</t>
-  </si>
-  <si>
-    <t>5y3q</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE CONJUGATED WITH BETA-MERCAPTOETHANOL</t>
-  </si>
-  <si>
-    <t>2017-07-29</t>
-  </si>
-  <si>
-    <t>2fe8</t>
-  </si>
-  <si>
-    <t>SARS CORONAVIRUS PAPAIN-LIKE PROTEASE: STRUCTURE OF A VIRAL DEUBIQUITINATING ENZYME</t>
-  </si>
-  <si>
-    <t>2005-12-15</t>
-  </si>
-  <si>
     <t>4ow0</t>
   </si>
   <si>
     <t>2014-01-28</t>
   </si>
   <si>
-    <t>5y3e</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE IN COMPLEX WITH GLYCEROL</t>
-  </si>
-  <si>
-    <t>2017-07-28</t>
-  </si>
-  <si>
-    <t>5e6j</t>
-  </si>
-  <si>
-    <t>STRUCTURE OF SARS PLPRO BOUND TO A LYS48-LINKED DI-UBIQUITIN ACTIVITY BASED PROBE</t>
-  </si>
-  <si>
-    <t>2015-10-09</t>
-  </si>
-  <si>
-    <t>4mm3</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH UBIQUITIN ALDEHYDE</t>
-  </si>
-  <si>
-    <t>2013-09-08</t>
-  </si>
-  <si>
-    <t>5tl7</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH C- TERMINAL DOMAIN MOUSE ISG15</t>
+    <t>2kaf</t>
+  </si>
+  <si>
+    <t>SOLUTION STRUCTURE OF THE SARS-UNIQUE DOMAIN-C FROM THE NONSTRUCTURAL PROTEIN 3 (NSP3) OF THE SEVERE ACUTE RESPIRATORY SYNDROME CORONAVIRUS</t>
+  </si>
+  <si>
+    <t>2008-11-05</t>
+  </si>
+  <si>
+    <t>2kqw</t>
+  </si>
+  <si>
+    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. II: STRUCTURE OF THE SUD-C DOMAIN OF SUD-MC</t>
+  </si>
+  <si>
+    <t>2009-11-19</t>
   </si>
   <si>
     <t>2jze</t>
@@ -177,15 +206,6 @@
     <t>2008-01-04</t>
   </si>
   <si>
-    <t>2w2g</t>
-  </si>
-  <si>
-    <t>HUMAN SARS CORONAVIRUS UNIQUE DOMAIN</t>
-  </si>
-  <si>
-    <t>2008-10-30</t>
-  </si>
-  <si>
     <t>2jzd</t>
   </si>
   <si>
@@ -207,6 +227,39 @@
     <t>NMR CONFORMER CLOSEST TO THE MEAN COORDINATES OF THE DOMAIN 513-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
   </si>
   <si>
+    <t>2kqv</t>
+  </si>
+  <si>
+    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. I: STRUCTURE OF THE SUD-M DOMAIN OF SUD-MC</t>
+  </si>
+  <si>
+    <t>2k87</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF A PUTATIVE RNA BINDING PROTEIN (SARS1) FROM SARS CORONAVIRUS</t>
+  </si>
+  <si>
+    <t>2008-09-02</t>
+  </si>
+  <si>
+    <t>2fav</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS MACRO DOMAIN IN COMPLEX WITH ADP- RIBOSE AT 1.8 A RESOLUTION</t>
+  </si>
+  <si>
+    <t>2005-12-08</t>
+  </si>
+  <si>
+    <t>2acf</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF SARS-COV NON-STRUCTURAL PROTEIN NSP3A (SARS1) FROM SARS CORONAVIRUS</t>
+  </si>
+  <si>
+    <t>2005-07-18</t>
+  </si>
+  <si>
     <t>2wct</t>
   </si>
   <si>
@@ -214,57 +267,6 @@
   </si>
   <si>
     <t>2009-03-16</t>
-  </si>
-  <si>
-    <t>2kqv</t>
-  </si>
-  <si>
-    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. I: STRUCTURE OF THE SUD-M DOMAIN OF SUD-MC</t>
-  </si>
-  <si>
-    <t>2009-11-19</t>
-  </si>
-  <si>
-    <t>2k87</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF A PUTATIVE RNA BINDING PROTEIN (SARS1) FROM SARS CORONAVIRUS</t>
-  </si>
-  <si>
-    <t>2008-09-02</t>
-  </si>
-  <si>
-    <t>2fav</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS MACRO DOMAIN IN COMPLEX WITH ADP- RIBOSE AT 1.8 A RESOLUTION</t>
-  </si>
-  <si>
-    <t>2005-12-08</t>
-  </si>
-  <si>
-    <t>2acf</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF SARS-COV NON-STRUCTURAL PROTEIN NSP3A (SARS1) FROM SARS CORONAVIRUS</t>
-  </si>
-  <si>
-    <t>2005-07-18</t>
-  </si>
-  <si>
-    <t>2kaf</t>
-  </si>
-  <si>
-    <t>SOLUTION STRUCTURE OF THE SARS-UNIQUE DOMAIN-C FROM THE NONSTRUCTURAL PROTEIN 3 (NSP3) OF THE SEVERE ACUTE RESPIRATORY SYNDROME CORONAVIRUS</t>
-  </si>
-  <si>
-    <t>2008-11-05</t>
-  </si>
-  <si>
-    <t>2kqw</t>
-  </si>
-  <si>
-    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. II: STRUCTURE OF THE SUD-C DOMAIN OF SUD-MC</t>
   </si>
 </sst>
 </file>
@@ -596,7 +598,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -663,16 +665,33 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.22</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
-        <v>14</v>
+      <c r="E5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -682,7 +701,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -712,206 +731,155 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>1.4</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>2.62</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>2.5</v>
+        <v>2.63</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5">
-        <v>2.5</v>
+        <v>1.65</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>2.63</v>
+        <v>1.85</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>1.65</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8">
-        <v>1.85</v>
+        <v>2.85</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B9">
-        <v>2.1</v>
+        <v>2.75</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <v>1.65</v>
+        <v>2.44</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11">
-        <v>2.85</v>
-      </c>
-      <c r="C11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>2.75</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13">
-        <v>2.44</v>
-      </c>
-      <c r="C13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +889,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -951,50 +919,50 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B3">
-        <v>2.22</v>
+        <v>2.5</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="C4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>51</v>
@@ -1002,70 +970,36 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7">
-        <v>2.79</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1074,6 +1008,126 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1105,19 +1159,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1125,9 +1179,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1157,36 +1211,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>1.8</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3">
-        <v>1.4</v>
-      </c>
-      <c r="C3" t="s">
         <v>75</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1194,9 +1231,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1226,36 +1263,71 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2">
+        <v>1.4</v>
+      </c>
+      <c r="C2" t="s">
         <v>77</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
       <c r="B2">
-        <v>0</v>
+        <v>2.79</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved domain classifier, extended domain information for SARS-CoV Nsp3
</commit_message>
<xml_diff>
--- a/pdb/nsp3/SARS-CoV/domains_and_infos_of_nsp3.xlsx
+++ b/pdb/nsp3/SARS-CoV/domains_and_infos_of_nsp3.xlsx
@@ -8,20 +8,22 @@
   </bookViews>
   <sheets>
     <sheet name="nsp3_Ubl1" sheetId="1" r:id="rId1"/>
-    <sheet name="nsp3_PL2pro" sheetId="2" r:id="rId2"/>
+    <sheet name="nsp3_Ubl2+PL2pro" sheetId="2" r:id="rId2"/>
     <sheet name="nsp3_Ubl2" sheetId="3" r:id="rId3"/>
-    <sheet name="nsp3_SUD" sheetId="4" r:id="rId4"/>
+    <sheet name="nsp3_Macro3" sheetId="4" r:id="rId4"/>
     <sheet name="nsp3_NAB" sheetId="5" r:id="rId5"/>
-    <sheet name="nsp3_sec_btwn_Macro1_SUD" sheetId="6" r:id="rId6"/>
-    <sheet name="nsp3_Macro1" sheetId="7" r:id="rId7"/>
-    <sheet name="nsp3_frgmnt_btwn_PL2pro_NAB" sheetId="8" r:id="rId8"/>
+    <sheet name="nsp3_LINKER-Mac1-Mac2" sheetId="6" r:id="rId6"/>
+    <sheet name="nsp3_Macro2" sheetId="7" r:id="rId7"/>
+    <sheet name="nsp3_Macro1" sheetId="8" r:id="rId8"/>
+    <sheet name="nsp3_DPUP" sheetId="9" r:id="rId9"/>
+    <sheet name="Organisms" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="91">
   <si>
     <t>PDB</t>
   </si>
@@ -50,15 +52,180 @@
     <t>2006-04-24</t>
   </si>
   <si>
+    <t>2idy</t>
+  </si>
+  <si>
+    <t>2006-09-15</t>
+  </si>
+  <si>
+    <t>4m0w</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE C112S MUTANT IN COMPLEX WITH UBIQUITIN</t>
+  </si>
+  <si>
+    <t>X-RAY DIFFRACTION</t>
+  </si>
+  <si>
+    <t>2013-08-02</t>
+  </si>
+  <si>
+    <t>5tl6</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH THE C-TERMINAL DOMAIN OF HUMAN ISG15</t>
+  </si>
+  <si>
+    <t>2016-10-10</t>
+  </si>
+  <si>
+    <t>3mj5</t>
+  </si>
+  <si>
+    <t>SEVERE ACUTE RESPIRATORY SYNDROME-CORONAVIRUS PAPAIN-LIKE PROTEASE INHIBITORS: DESIGN, SYNTHESIS, PROTEIN-LIGAND X-RAY STRUCTURE AND BIOLOGICAL EVALUATION</t>
+  </si>
+  <si>
+    <t>2010-04-12</t>
+  </si>
+  <si>
+    <t>5y3q</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE CONJUGATED WITH BETA-MERCAPTOETHANOL</t>
+  </si>
+  <si>
+    <t>2017-07-29</t>
+  </si>
+  <si>
+    <t>2fe8</t>
+  </si>
+  <si>
+    <t>SARS CORONAVIRUS PAPAIN-LIKE PROTEASE: STRUCTURE OF A VIRAL DEUBIQUITINATING ENZYME</t>
+  </si>
+  <si>
+    <t>2005-12-15</t>
+  </si>
+  <si>
+    <t>5y3e</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE IN COMPLEX WITH GLYCEROL</t>
+  </si>
+  <si>
+    <t>2017-07-28</t>
+  </si>
+  <si>
+    <t>5e6j</t>
+  </si>
+  <si>
+    <t>STRUCTURE OF SARS PLPRO BOUND TO A LYS48-LINKED DI-UBIQUITIN ACTIVITY BASED PROBE</t>
+  </si>
+  <si>
+    <t>2015-10-09</t>
+  </si>
+  <si>
+    <t>4mm3</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH UBIQUITIN ALDEHYDE</t>
+  </si>
+  <si>
+    <t>2013-09-08</t>
+  </si>
+  <si>
+    <t>5tl7</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH C- TERMINAL DOMAIN MOUSE ISG15</t>
+  </si>
+  <si>
+    <t>3e9s</t>
+  </si>
+  <si>
+    <t>A NEW CLASS OF PAPAIN-LIKE PROTEASE/DEUBIQUITINASE INHIBITORS BLOCKS SARS VIRUS REPLICATION</t>
+  </si>
+  <si>
+    <t>2008-08-23</t>
+  </si>
+  <si>
+    <t>4ovz</t>
+  </si>
+  <si>
+    <t>X-RAY STRUCTURAL AND BIOLOGICAL EVALUATION OF A SERIES OF POTENT AND HIGHLY SELECTIVE INHIBITORS OF HUMAN CORONAVIRUS PAPAIN-LIKE PROTEASES</t>
+  </si>
+  <si>
+    <t>2014-01-27</t>
+  </si>
+  <si>
+    <t>4ow0</t>
+  </si>
+  <si>
+    <t>2014-01-28</t>
+  </si>
+  <si>
+    <t>2jze</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF THE DOMAIN 527-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3, SINGLE CONFORMER CLOSEST TO THE MEAN COORDINATES OF AN ENSEMBLE OF TWENTY ENERGY MINIMIZED CONFORMERS</t>
+  </si>
+  <si>
+    <t>2008-01-04</t>
+  </si>
+  <si>
+    <t>2jzd</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF THE DOMAIN 527-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
+  </si>
+  <si>
+    <t>2rnk</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF THE DOMAIN 513-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
+  </si>
+  <si>
+    <t>2008-01-11</t>
+  </si>
+  <si>
+    <t>2jzf</t>
+  </si>
+  <si>
+    <t>NMR CONFORMER CLOSEST TO THE MEAN COORDINATES OF THE DOMAIN 513-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
+  </si>
+  <si>
+    <t>2kqv</t>
+  </si>
+  <si>
+    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. I: STRUCTURE OF THE SUD-M DOMAIN OF SUD-MC</t>
+  </si>
+  <si>
+    <t>2009-11-19</t>
+  </si>
+  <si>
+    <t>2k87</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF A PUTATIVE RNA BINDING PROTEIN (SARS1) FROM SARS CORONAVIRUS</t>
+  </si>
+  <si>
+    <t>2008-09-02</t>
+  </si>
+  <si>
+    <t>2fav</t>
+  </si>
+  <si>
+    <t>CRYSTAL STRUCTURE OF SARS MACRO DOMAIN IN COMPLEX WITH ADP- RIBOSE AT 1.8 A RESOLUTION</t>
+  </si>
+  <si>
+    <t>2005-12-08</t>
+  </si>
+  <si>
     <t>6yxj</t>
   </si>
   <si>
     <t>CRYSTAL STRUCTURE OF SARS-COV MACRODOMAIN II IN COMPLEX WITH HUMAN PAIP1</t>
   </si>
   <si>
-    <t>X-RAY DIFFRACTION</t>
-  </si>
-  <si>
     <t>2020-05-02</t>
   </si>
   <si>
@@ -71,112 +238,22 @@
     <t>2008-10-30</t>
   </si>
   <si>
-    <t>2idy</t>
-  </si>
-  <si>
-    <t>2006-09-15</t>
-  </si>
-  <si>
-    <t>4m0w</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE C112S MUTANT IN COMPLEX WITH UBIQUITIN</t>
-  </si>
-  <si>
-    <t>2013-08-02</t>
-  </si>
-  <si>
-    <t>5tl6</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH THE C-TERMINAL DOMAIN OF HUMAN ISG15</t>
-  </si>
-  <si>
-    <t>2016-10-10</t>
-  </si>
-  <si>
-    <t>3mj5</t>
-  </si>
-  <si>
-    <t>SEVERE ACUTE RESPIRATORY SYNDROME-CORONAVIRUS PAPAIN-LIKE PROTEASE INHIBITORS: DESIGN, SYNTHESIS, PROTEIN-LIGAND X-RAY STRUCTURE AND BIOLOGICAL EVALUATION</t>
-  </si>
-  <si>
-    <t>2010-04-12</t>
-  </si>
-  <si>
-    <t>5y3q</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE CONJUGATED WITH BETA-MERCAPTOETHANOL</t>
-  </si>
-  <si>
-    <t>2017-07-29</t>
-  </si>
-  <si>
-    <t>2fe8</t>
-  </si>
-  <si>
-    <t>SARS CORONAVIRUS PAPAIN-LIKE PROTEASE: STRUCTURE OF A VIRAL DEUBIQUITINATING ENZYME</t>
-  </si>
-  <si>
-    <t>2005-12-15</t>
-  </si>
-  <si>
-    <t>5y3e</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS CORONAVIRUS PAPAIN-LIKE PROTEASE IN COMPLEX WITH GLYCEROL</t>
-  </si>
-  <si>
-    <t>2017-07-28</t>
-  </si>
-  <si>
-    <t>5e6j</t>
-  </si>
-  <si>
-    <t>STRUCTURE OF SARS PLPRO BOUND TO A LYS48-LINKED DI-UBIQUITIN ACTIVITY BASED PROBE</t>
-  </si>
-  <si>
-    <t>2015-10-09</t>
-  </si>
-  <si>
-    <t>4mm3</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE PLPRO IN COMPLEX WITH UBIQUITIN ALDEHYDE</t>
-  </si>
-  <si>
-    <t>2013-09-08</t>
-  </si>
-  <si>
-    <t>5tl7</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS-COV PAPAIN-LIKE PROTEASE IN COMPLEX WITH C- TERMINAL DOMAIN MOUSE ISG15</t>
-  </si>
-  <si>
-    <t>3e9s</t>
-  </si>
-  <si>
-    <t>A NEW CLASS OF PAPAIN-LIKE PROTEASE/DEUBIQUITINASE INHIBITORS BLOCKS SARS VIRUS REPLICATION</t>
-  </si>
-  <si>
-    <t>2008-08-23</t>
-  </si>
-  <si>
-    <t>4ovz</t>
-  </si>
-  <si>
-    <t>X-RAY STRUCTURAL AND BIOLOGICAL EVALUATION OF A SERIES OF POTENT AND HIGHLY SELECTIVE INHIBITORS OF HUMAN CORONAVIRUS PAPAIN-LIKE PROTEASES</t>
-  </si>
-  <si>
-    <t>2014-01-27</t>
-  </si>
-  <si>
-    <t>4ow0</t>
-  </si>
-  <si>
-    <t>2014-01-28</t>
+    <t>2wct</t>
+  </si>
+  <si>
+    <t>HUMAN SARS CORONAVIRUS UNIQUE DOMAIN (TRICLINIC FORM)</t>
+  </si>
+  <si>
+    <t>2009-03-16</t>
+  </si>
+  <si>
+    <t>2acf</t>
+  </si>
+  <si>
+    <t>NMR STRUCTURE OF SARS-COV NON-STRUCTURAL PROTEIN NSP3A (SARS1) FROM SARS CORONAVIRUS</t>
+  </si>
+  <si>
+    <t>2005-07-18</t>
   </si>
   <si>
     <t>2kaf</t>
@@ -194,79 +271,31 @@
     <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. II: STRUCTURE OF THE SUD-C DOMAIN OF SUD-MC</t>
   </si>
   <si>
-    <t>2009-11-19</t>
-  </si>
-  <si>
-    <t>2jze</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF THE DOMAIN 527-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3, SINGLE CONFORMER CLOSEST TO THE MEAN COORDINATES OF AN ENSEMBLE OF TWENTY ENERGY MINIMIZED CONFORMERS</t>
-  </si>
-  <si>
-    <t>2008-01-04</t>
-  </si>
-  <si>
-    <t>2jzd</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF THE DOMAIN 527-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
-  </si>
-  <si>
-    <t>2rnk</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF THE DOMAIN 513-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
-  </si>
-  <si>
-    <t>2008-01-11</t>
-  </si>
-  <si>
-    <t>2jzf</t>
-  </si>
-  <si>
-    <t>NMR CONFORMER CLOSEST TO THE MEAN COORDINATES OF THE DOMAIN 513-651 OF THE SARS-COV NONSTRUCTURAL PROTEIN NSP3</t>
-  </si>
-  <si>
-    <t>2kqv</t>
-  </si>
-  <si>
-    <t>SARS CORONAVIRUS-UNIQUE DOMAIN (SUD): THREE-DOMAIN MOLECULAR ARCHITECTURE IN SOLUTION AND RNA BINDING. I: STRUCTURE OF THE SUD-M DOMAIN OF SUD-MC</t>
-  </si>
-  <si>
-    <t>2k87</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF A PUTATIVE RNA BINDING PROTEIN (SARS1) FROM SARS CORONAVIRUS</t>
-  </si>
-  <si>
-    <t>2008-09-02</t>
-  </si>
-  <si>
-    <t>2fav</t>
-  </si>
-  <si>
-    <t>CRYSTAL STRUCTURE OF SARS MACRO DOMAIN IN COMPLEX WITH ADP- RIBOSE AT 1.8 A RESOLUTION</t>
-  </si>
-  <si>
-    <t>2005-12-08</t>
-  </si>
-  <si>
-    <t>2acf</t>
-  </si>
-  <si>
-    <t>NMR STRUCTURE OF SARS-COV NON-STRUCTURAL PROTEIN NSP3A (SARS1) FROM SARS CORONAVIRUS</t>
-  </si>
-  <si>
-    <t>2005-07-18</t>
-  </si>
-  <si>
-    <t>2wct</t>
-  </si>
-  <si>
-    <t>HUMAN SARS CORONAVIRUS UNIQUE DOMAIN (TRICLINIC FORM)</t>
-  </si>
-  <si>
-    <t>2009-03-16</t>
+    <t>Lists all PDBs which contain sequences of a certain organism.</t>
+  </si>
+  <si>
+    <t>Organism</t>
+  </si>
+  <si>
+    <t>sars coronavirus</t>
+  </si>
+  <si>
+    <t>bos taurus</t>
+  </si>
+  <si>
+    <t>human sars coronavirus</t>
+  </si>
+  <si>
+    <t>homo sapiens</t>
+  </si>
+  <si>
+    <t>severe acute respiratory syndrome coronavirus</t>
+  </si>
+  <si>
+    <t>sars coronavirus tor2</t>
+  </si>
+  <si>
+    <t>mus musculus</t>
   </si>
 </sst>
 </file>
@@ -598,7 +627,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -648,50 +677,241 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>2.22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
+    <row r="29" spans="1:2">
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -731,155 +951,155 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1.4</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>2.62</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>2.63</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>1.65</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>1.85</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>1.65</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>2.85</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>2.75</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>2.44</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -889,7 +1109,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -919,87 +1139,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>2.5</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B3">
         <v>2.5</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>2.1</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1039,87 +1225,87 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1159,19 +1345,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1211,19 +1397,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <v>1.8</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +1419,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1263,19 +1449,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B2">
-        <v>1.4</v>
+        <v>3.5</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3">
+        <v>2.22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>2.79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1315,19 +1535,88 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <v>1.4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="110.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>79</v>
       </c>
-      <c r="B2">
-        <v>2.79</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>80</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>81</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>